<commit_message>
made a starting point for report
</commit_message>
<xml_diff>
--- a/recursive_map.xlsx
+++ b/recursive_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Custom_Projects\optimering_grupp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFD2037-3778-4DF7-B914-A5A8D2F3FDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65322A-09F6-45ED-BC69-3BCDF2E20AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E2015ED8-7778-4B4B-B55F-488E888CCD57}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,14 +94,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,14 +258,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
@@ -365,16 +356,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -389,30 +377,32 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="40% - Accent2" xfId="7" builtinId="35"/>
+  <cellStyles count="7">
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
-    <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Linked Cell" xfId="5" builtinId="24"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -1058,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D49F0B6-0387-4E66-8DC6-56828B3094F0}">
   <dimension ref="B1:CL124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O82" sqref="O82"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AL29" sqref="AL29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1511,7 +1501,7 @@
       <c r="E15" s="10">
         <v>0</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="20">
         <v>6</v>
       </c>
       <c r="G15" s="12">
@@ -1538,7 +1528,7 @@
       <c r="O15" s="10">
         <v>0</v>
       </c>
-      <c r="P15" s="11">
+      <c r="P15" s="20">
         <v>6</v>
       </c>
       <c r="Q15" s="12">
@@ -1564,13 +1554,13 @@
       <c r="D16" s="15">
         <v>0</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="21">
         <v>8</v>
       </c>
       <c r="F16" s="14">
         <v>0</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="25">
         <v>3</v>
       </c>
       <c r="H16" s="13">
@@ -1591,13 +1581,13 @@
       <c r="N16" s="15">
         <v>0</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="21">
         <v>8</v>
       </c>
       <c r="P16" s="14">
         <v>0</v>
       </c>
-      <c r="Q16" s="15">
+      <c r="Q16" s="25">
         <v>3</v>
       </c>
       <c r="R16" s="13">
@@ -1623,7 +1613,7 @@
       <c r="E17" s="16">
         <v>0</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="22">
         <v>2</v>
       </c>
       <c r="G17" s="18">
@@ -1650,7 +1640,7 @@
       <c r="O17" s="16">
         <v>0</v>
       </c>
-      <c r="P17" s="17">
+      <c r="P17" s="22">
         <v>2</v>
       </c>
       <c r="Q17" s="18">
@@ -1869,7 +1859,7 @@
       <c r="M23" s="20">
         <v>3</v>
       </c>
-      <c r="N23" s="38">
+      <c r="N23" s="37">
         <v>1</v>
       </c>
       <c r="O23" s="32">
@@ -2097,7 +2087,7 @@
       <c r="E26" s="10">
         <v>0</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="20">
         <v>6</v>
       </c>
       <c r="G26" s="12">
@@ -2124,7 +2114,7 @@
       <c r="O26" s="10">
         <v>0</v>
       </c>
-      <c r="P26" s="11">
+      <c r="P26" s="20">
         <v>6</v>
       </c>
       <c r="Q26" s="12">
@@ -2151,7 +2141,7 @@
       <c r="Y26" s="10">
         <v>0</v>
       </c>
-      <c r="Z26" s="11">
+      <c r="Z26" s="20">
         <v>6</v>
       </c>
       <c r="AA26" s="12">
@@ -2177,13 +2167,13 @@
       <c r="D27" s="15">
         <v>0</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="21">
         <v>8</v>
       </c>
       <c r="F27" s="14">
         <v>0</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="25">
         <v>3</v>
       </c>
       <c r="H27" s="13">
@@ -2204,13 +2194,13 @@
       <c r="N27" s="15">
         <v>0</v>
       </c>
-      <c r="O27" s="13">
+      <c r="O27" s="21">
         <v>8</v>
       </c>
       <c r="P27" s="14">
         <v>0</v>
       </c>
-      <c r="Q27" s="15">
+      <c r="Q27" s="25">
         <v>3</v>
       </c>
       <c r="R27" s="13">
@@ -2231,13 +2221,13 @@
       <c r="X27" s="15">
         <v>0</v>
       </c>
-      <c r="Y27" s="13">
+      <c r="Y27" s="21">
         <v>8</v>
       </c>
       <c r="Z27" s="14">
         <v>0</v>
       </c>
-      <c r="AA27" s="15">
+      <c r="AA27" s="25">
         <v>3</v>
       </c>
       <c r="AB27" s="13">
@@ -2263,7 +2253,7 @@
       <c r="E28" s="16">
         <v>0</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="22">
         <v>2</v>
       </c>
       <c r="G28" s="18">
@@ -2290,7 +2280,7 @@
       <c r="O28" s="16">
         <v>0</v>
       </c>
-      <c r="P28" s="17">
+      <c r="P28" s="22">
         <v>2</v>
       </c>
       <c r="Q28" s="18">
@@ -2317,7 +2307,7 @@
       <c r="Y28" s="16">
         <v>0</v>
       </c>
-      <c r="Z28" s="17">
+      <c r="Z28" s="22">
         <v>2</v>
       </c>
       <c r="AA28" s="18">
@@ -2617,7 +2607,7 @@
       <c r="M34" s="20">
         <v>3</v>
       </c>
-      <c r="N34" s="38">
+      <c r="N34" s="37">
         <v>1</v>
       </c>
       <c r="O34" s="29">
@@ -2647,7 +2637,7 @@
       <c r="X34" s="28">
         <v>1</v>
       </c>
-      <c r="Y34" s="42">
+      <c r="Y34" s="41">
         <v>2</v>
       </c>
       <c r="Z34" s="20">
@@ -2668,7 +2658,7 @@
       <c r="AF34" s="19">
         <v>5</v>
       </c>
-      <c r="AG34" s="43">
+      <c r="AG34" s="42">
         <v>3</v>
       </c>
       <c r="AH34" s="28">
@@ -3007,7 +2997,7 @@
       <c r="E37" s="10">
         <v>0</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F37" s="20">
         <v>6</v>
       </c>
       <c r="G37" s="12">
@@ -3034,7 +3024,7 @@
       <c r="O37" s="10">
         <v>0</v>
       </c>
-      <c r="P37" s="11">
+      <c r="P37" s="20">
         <v>6</v>
       </c>
       <c r="Q37" s="12">
@@ -3061,7 +3051,7 @@
       <c r="Y37" s="10">
         <v>0</v>
       </c>
-      <c r="Z37" s="11">
+      <c r="Z37" s="20">
         <v>6</v>
       </c>
       <c r="AA37" s="12">
@@ -3088,7 +3078,7 @@
       <c r="AI37" s="10">
         <v>0</v>
       </c>
-      <c r="AJ37" s="11">
+      <c r="AJ37" s="20">
         <v>6</v>
       </c>
       <c r="AK37" s="12">
@@ -3115,7 +3105,7 @@
       <c r="AS37" s="10">
         <v>0</v>
       </c>
-      <c r="AT37" s="11">
+      <c r="AT37" s="20">
         <v>6</v>
       </c>
       <c r="AU37" s="12">
@@ -3141,13 +3131,13 @@
       <c r="D38" s="15">
         <v>0</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="21">
         <v>8</v>
       </c>
       <c r="F38" s="14">
         <v>0</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="25">
         <v>3</v>
       </c>
       <c r="H38" s="13">
@@ -3168,13 +3158,13 @@
       <c r="N38" s="15">
         <v>0</v>
       </c>
-      <c r="O38" s="13">
+      <c r="O38" s="21">
         <v>8</v>
       </c>
       <c r="P38" s="14">
         <v>0</v>
       </c>
-      <c r="Q38" s="15">
+      <c r="Q38" s="25">
         <v>3</v>
       </c>
       <c r="R38" s="13">
@@ -3195,13 +3185,13 @@
       <c r="X38" s="15">
         <v>0</v>
       </c>
-      <c r="Y38" s="13">
+      <c r="Y38" s="21">
         <v>8</v>
       </c>
       <c r="Z38" s="14">
         <v>0</v>
       </c>
-      <c r="AA38" s="15">
+      <c r="AA38" s="25">
         <v>3</v>
       </c>
       <c r="AB38" s="13">
@@ -3222,13 +3212,13 @@
       <c r="AH38" s="15">
         <v>0</v>
       </c>
-      <c r="AI38" s="13">
+      <c r="AI38" s="21">
         <v>8</v>
       </c>
       <c r="AJ38" s="14">
         <v>0</v>
       </c>
-      <c r="AK38" s="33">
+      <c r="AK38" s="43">
         <v>3</v>
       </c>
       <c r="AL38" s="13">
@@ -3249,13 +3239,13 @@
       <c r="AR38" s="15">
         <v>0</v>
       </c>
-      <c r="AS38" s="13">
+      <c r="AS38" s="21">
         <v>8</v>
       </c>
       <c r="AT38" s="14">
         <v>0</v>
       </c>
-      <c r="AU38" s="15">
+      <c r="AU38" s="25">
         <v>3</v>
       </c>
       <c r="AV38" s="13">
@@ -3281,7 +3271,7 @@
       <c r="E39" s="16">
         <v>0</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="22">
         <v>2</v>
       </c>
       <c r="G39" s="18">
@@ -3308,7 +3298,7 @@
       <c r="O39" s="16">
         <v>0</v>
       </c>
-      <c r="P39" s="17">
+      <c r="P39" s="22">
         <v>2</v>
       </c>
       <c r="Q39" s="18">
@@ -3335,7 +3325,7 @@
       <c r="Y39" s="16">
         <v>0</v>
       </c>
-      <c r="Z39" s="17">
+      <c r="Z39" s="22">
         <v>2</v>
       </c>
       <c r="AA39" s="18">
@@ -3362,7 +3352,7 @@
       <c r="AI39" s="16">
         <v>0</v>
       </c>
-      <c r="AJ39" s="17">
+      <c r="AJ39" s="22">
         <v>2</v>
       </c>
       <c r="AK39" s="18">
@@ -3389,7 +3379,7 @@
       <c r="AS39" s="16">
         <v>0</v>
       </c>
-      <c r="AT39" s="17">
+      <c r="AT39" s="22">
         <v>2</v>
       </c>
       <c r="AU39" s="18">
@@ -3851,7 +3841,7 @@
       <c r="M45" s="20">
         <v>3</v>
       </c>
-      <c r="N45" s="38">
+      <c r="N45" s="37">
         <v>1</v>
       </c>
       <c r="O45" s="29">
@@ -3881,7 +3871,7 @@
       <c r="X45" s="28">
         <v>1</v>
       </c>
-      <c r="Y45" s="42">
+      <c r="Y45" s="41">
         <v>2</v>
       </c>
       <c r="Z45" s="20">
@@ -3902,7 +3892,7 @@
       <c r="AF45" s="19">
         <v>5</v>
       </c>
-      <c r="AG45" s="43">
+      <c r="AG45" s="42">
         <v>3</v>
       </c>
       <c r="AH45" s="28">
@@ -3941,7 +3931,7 @@
       <c r="AT45" s="20">
         <v>7</v>
       </c>
-      <c r="AU45" s="38">
+      <c r="AU45" s="37">
         <v>4</v>
       </c>
       <c r="AV45" s="32">
@@ -3953,7 +3943,7 @@
       <c r="AX45" s="12">
         <v>0</v>
       </c>
-      <c r="AZ45" s="42">
+      <c r="AZ45" s="41">
         <v>5</v>
       </c>
       <c r="BA45" s="20">
@@ -4019,7 +4009,7 @@
       <c r="BW45" s="29">
         <v>2</v>
       </c>
-      <c r="BX45" s="43">
+      <c r="BX45" s="42">
         <v>7</v>
       </c>
       <c r="BY45" s="28">
@@ -4491,7 +4481,7 @@
       <c r="BP47" s="16">
         <v>0</v>
       </c>
-      <c r="BQ47" s="40">
+      <c r="BQ47" s="39">
         <v>6</v>
       </c>
       <c r="BR47" s="18">
@@ -4565,7 +4555,7 @@
       <c r="E48" s="10">
         <v>0</v>
       </c>
-      <c r="F48" s="11">
+      <c r="F48" s="20">
         <v>6</v>
       </c>
       <c r="G48" s="12">
@@ -4592,7 +4582,7 @@
       <c r="O48" s="10">
         <v>0</v>
       </c>
-      <c r="P48" s="11">
+      <c r="P48" s="20">
         <v>6</v>
       </c>
       <c r="Q48" s="12">
@@ -4619,7 +4609,7 @@
       <c r="Y48" s="10">
         <v>0</v>
       </c>
-      <c r="Z48" s="11">
+      <c r="Z48" s="20">
         <v>6</v>
       </c>
       <c r="AA48" s="12">
@@ -4646,7 +4636,7 @@
       <c r="AI48" s="10">
         <v>0</v>
       </c>
-      <c r="AJ48" s="11">
+      <c r="AJ48" s="20">
         <v>6</v>
       </c>
       <c r="AK48" s="12">
@@ -4673,7 +4663,7 @@
       <c r="AS48" s="10">
         <v>0</v>
       </c>
-      <c r="AT48" s="11">
+      <c r="AT48" s="20">
         <v>6</v>
       </c>
       <c r="AU48" s="12">
@@ -4700,7 +4690,7 @@
       <c r="BC48" s="10">
         <v>0</v>
       </c>
-      <c r="BD48" s="11">
+      <c r="BD48" s="20">
         <v>6</v>
       </c>
       <c r="BE48" s="12">
@@ -4727,7 +4717,7 @@
       <c r="BM48" s="10">
         <v>0</v>
       </c>
-      <c r="BN48" s="11">
+      <c r="BN48" s="20">
         <v>6</v>
       </c>
       <c r="BO48" s="12">
@@ -4754,7 +4744,7 @@
       <c r="BW48" s="10">
         <v>0</v>
       </c>
-      <c r="BX48" s="11">
+      <c r="BX48" s="20">
         <v>6</v>
       </c>
       <c r="BY48" s="12">
@@ -4781,7 +4771,7 @@
       <c r="CG48" s="10">
         <v>0</v>
       </c>
-      <c r="CH48" s="11">
+      <c r="CH48" s="20">
         <v>6</v>
       </c>
       <c r="CI48" s="12">
@@ -4807,13 +4797,13 @@
       <c r="D49" s="15">
         <v>0</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49" s="21">
         <v>8</v>
       </c>
       <c r="F49" s="14">
         <v>0</v>
       </c>
-      <c r="G49" s="15">
+      <c r="G49" s="25">
         <v>3</v>
       </c>
       <c r="H49" s="13">
@@ -4834,13 +4824,13 @@
       <c r="N49" s="15">
         <v>0</v>
       </c>
-      <c r="O49" s="13">
+      <c r="O49" s="21">
         <v>8</v>
       </c>
       <c r="P49" s="14">
         <v>0</v>
       </c>
-      <c r="Q49" s="15">
+      <c r="Q49" s="25">
         <v>3</v>
       </c>
       <c r="R49" s="13">
@@ -4861,13 +4851,13 @@
       <c r="X49" s="15">
         <v>0</v>
       </c>
-      <c r="Y49" s="13">
+      <c r="Y49" s="21">
         <v>8</v>
       </c>
       <c r="Z49" s="14">
         <v>0</v>
       </c>
-      <c r="AA49" s="15">
+      <c r="AA49" s="25">
         <v>3</v>
       </c>
       <c r="AB49" s="13">
@@ -4888,13 +4878,13 @@
       <c r="AH49" s="15">
         <v>0</v>
       </c>
-      <c r="AI49" s="13">
+      <c r="AI49" s="21">
         <v>8</v>
       </c>
       <c r="AJ49" s="14">
         <v>0</v>
       </c>
-      <c r="AK49" s="15">
+      <c r="AK49" s="25">
         <v>3</v>
       </c>
       <c r="AL49" s="13">
@@ -4915,13 +4905,13 @@
       <c r="AR49" s="15">
         <v>0</v>
       </c>
-      <c r="AS49" s="13">
+      <c r="AS49" s="21">
         <v>8</v>
       </c>
       <c r="AT49" s="14">
         <v>0</v>
       </c>
-      <c r="AU49" s="15">
+      <c r="AU49" s="25">
         <v>3</v>
       </c>
       <c r="AV49" s="13">
@@ -4942,13 +4932,13 @@
       <c r="BB49" s="15">
         <v>0</v>
       </c>
-      <c r="BC49" s="13">
+      <c r="BC49" s="21">
         <v>8</v>
       </c>
       <c r="BD49" s="14">
         <v>0</v>
       </c>
-      <c r="BE49" s="15">
+      <c r="BE49" s="25">
         <v>3</v>
       </c>
       <c r="BF49" s="13">
@@ -4969,13 +4959,13 @@
       <c r="BL49" s="15">
         <v>0</v>
       </c>
-      <c r="BM49" s="13">
+      <c r="BM49" s="21">
         <v>8</v>
       </c>
       <c r="BN49" s="14">
         <v>0</v>
       </c>
-      <c r="BO49" s="15">
+      <c r="BO49" s="25">
         <v>3</v>
       </c>
       <c r="BP49" s="13">
@@ -4996,13 +4986,13 @@
       <c r="BV49" s="15">
         <v>0</v>
       </c>
-      <c r="BW49" s="13">
+      <c r="BW49" s="21">
         <v>8</v>
       </c>
       <c r="BX49" s="14">
         <v>0</v>
       </c>
-      <c r="BY49" s="15">
+      <c r="BY49" s="25">
         <v>3</v>
       </c>
       <c r="BZ49" s="13">
@@ -5023,13 +5013,13 @@
       <c r="CF49" s="15">
         <v>0</v>
       </c>
-      <c r="CG49" s="13">
+      <c r="CG49" s="21">
         <v>8</v>
       </c>
       <c r="CH49" s="14">
         <v>0</v>
       </c>
-      <c r="CI49" s="15">
+      <c r="CI49" s="25">
         <v>3</v>
       </c>
       <c r="CJ49" s="13">
@@ -5055,7 +5045,7 @@
       <c r="E50" s="16">
         <v>0</v>
       </c>
-      <c r="F50" s="17">
+      <c r="F50" s="22">
         <v>2</v>
       </c>
       <c r="G50" s="18">
@@ -5082,7 +5072,7 @@
       <c r="O50" s="16">
         <v>0</v>
       </c>
-      <c r="P50" s="17">
+      <c r="P50" s="22">
         <v>2</v>
       </c>
       <c r="Q50" s="18">
@@ -5109,7 +5099,7 @@
       <c r="Y50" s="16">
         <v>0</v>
       </c>
-      <c r="Z50" s="17">
+      <c r="Z50" s="22">
         <v>2</v>
       </c>
       <c r="AA50" s="18">
@@ -5136,7 +5126,7 @@
       <c r="AI50" s="16">
         <v>0</v>
       </c>
-      <c r="AJ50" s="17">
+      <c r="AJ50" s="22">
         <v>2</v>
       </c>
       <c r="AK50" s="18">
@@ -5163,7 +5153,7 @@
       <c r="AS50" s="16">
         <v>0</v>
       </c>
-      <c r="AT50" s="17">
+      <c r="AT50" s="22">
         <v>2</v>
       </c>
       <c r="AU50" s="18">
@@ -5190,7 +5180,7 @@
       <c r="BC50" s="16">
         <v>0</v>
       </c>
-      <c r="BD50" s="17">
+      <c r="BD50" s="22">
         <v>2</v>
       </c>
       <c r="BE50" s="18">
@@ -5217,7 +5207,7 @@
       <c r="BM50" s="16">
         <v>0</v>
       </c>
-      <c r="BN50" s="17">
+      <c r="BN50" s="22">
         <v>2</v>
       </c>
       <c r="BO50" s="18">
@@ -5244,7 +5234,7 @@
       <c r="BW50" s="16">
         <v>0</v>
       </c>
-      <c r="BX50" s="17">
+      <c r="BX50" s="22">
         <v>2</v>
       </c>
       <c r="BY50" s="18">
@@ -5271,7 +5261,7 @@
       <c r="CG50" s="16">
         <v>0</v>
       </c>
-      <c r="CH50" s="17">
+      <c r="CH50" s="22">
         <v>2</v>
       </c>
       <c r="CI50" s="18">
@@ -6072,7 +6062,7 @@
       <c r="R56" s="29">
         <v>8</v>
       </c>
-      <c r="S56" s="35" t="s">
+      <c r="S56" s="34" t="s">
         <v>0</v>
       </c>
       <c r="T56" s="12">
@@ -6099,7 +6089,7 @@
       <c r="AB56" s="29">
         <v>8</v>
       </c>
-      <c r="AC56" s="34">
+      <c r="AC56" s="33">
         <v>9</v>
       </c>
       <c r="AD56" s="12">
@@ -6285,7 +6275,7 @@
       <c r="E59" s="10">
         <v>0</v>
       </c>
-      <c r="F59" s="11">
+      <c r="F59" s="20">
         <v>6</v>
       </c>
       <c r="G59" s="12">
@@ -6312,7 +6302,7 @@
       <c r="O59" s="10">
         <v>0</v>
       </c>
-      <c r="P59" s="11">
+      <c r="P59" s="20">
         <v>6</v>
       </c>
       <c r="Q59" s="12">
@@ -6339,7 +6329,7 @@
       <c r="Y59" s="10">
         <v>0</v>
       </c>
-      <c r="Z59" s="11">
+      <c r="Z59" s="20">
         <v>6</v>
       </c>
       <c r="AA59" s="12">
@@ -6365,13 +6355,13 @@
       <c r="D60" s="15">
         <v>0</v>
       </c>
-      <c r="E60" s="13">
+      <c r="E60" s="21">
         <v>8</v>
       </c>
       <c r="F60" s="14">
         <v>0</v>
       </c>
-      <c r="G60" s="15">
+      <c r="G60" s="25">
         <v>3</v>
       </c>
       <c r="H60" s="13">
@@ -6392,13 +6382,13 @@
       <c r="N60" s="15">
         <v>0</v>
       </c>
-      <c r="O60" s="13">
+      <c r="O60" s="21">
         <v>8</v>
       </c>
       <c r="P60" s="14">
         <v>0</v>
       </c>
-      <c r="Q60" s="15">
+      <c r="Q60" s="25">
         <v>3</v>
       </c>
       <c r="R60" s="13">
@@ -6419,13 +6409,13 @@
       <c r="X60" s="15">
         <v>0</v>
       </c>
-      <c r="Y60" s="13">
+      <c r="Y60" s="21">
         <v>8</v>
       </c>
       <c r="Z60" s="14">
         <v>0</v>
       </c>
-      <c r="AA60" s="15">
+      <c r="AA60" s="25">
         <v>3</v>
       </c>
       <c r="AB60" s="13">
@@ -6451,7 +6441,7 @@
       <c r="E61" s="16">
         <v>0</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="22">
         <v>2</v>
       </c>
       <c r="G61" s="18">
@@ -6478,7 +6468,7 @@
       <c r="O61" s="16">
         <v>0</v>
       </c>
-      <c r="P61" s="17">
+      <c r="P61" s="22">
         <v>2</v>
       </c>
       <c r="Q61" s="18">
@@ -6505,7 +6495,7 @@
       <c r="Y61" s="16">
         <v>0</v>
       </c>
-      <c r="Z61" s="17">
+      <c r="Z61" s="22">
         <v>2</v>
       </c>
       <c r="AA61" s="18">
@@ -6793,7 +6783,7 @@
       <c r="H67" s="29">
         <v>8</v>
       </c>
-      <c r="I67" s="34">
+      <c r="I67" s="33">
         <v>9</v>
       </c>
       <c r="J67" s="12">
@@ -6820,7 +6810,7 @@
       <c r="R67" s="29">
         <v>8</v>
       </c>
-      <c r="S67" s="34">
+      <c r="S67" s="33">
         <v>9</v>
       </c>
       <c r="T67" s="31" t="s">
@@ -6847,7 +6837,7 @@
       <c r="AB67" s="29">
         <v>8</v>
       </c>
-      <c r="AC67" s="34">
+      <c r="AC67" s="33">
         <v>9</v>
       </c>
       <c r="AD67" s="31">
@@ -7067,7 +7057,7 @@
       <c r="AB69" s="16">
         <v>0</v>
       </c>
-      <c r="AC69" s="40">
+      <c r="AC69" s="39">
         <v>6</v>
       </c>
       <c r="AD69" s="18">
@@ -7114,7 +7104,7 @@
       <c r="E70" s="10">
         <v>0</v>
       </c>
-      <c r="F70" s="11">
+      <c r="F70" s="20">
         <v>6</v>
       </c>
       <c r="G70" s="12">
@@ -7141,7 +7131,7 @@
       <c r="O70" s="10">
         <v>0</v>
       </c>
-      <c r="P70" s="11">
+      <c r="P70" s="20">
         <v>6</v>
       </c>
       <c r="Q70" s="12">
@@ -7168,7 +7158,7 @@
       <c r="Y70" s="10">
         <v>0</v>
       </c>
-      <c r="Z70" s="11">
+      <c r="Z70" s="20">
         <v>6</v>
       </c>
       <c r="AA70" s="12">
@@ -7195,7 +7185,7 @@
       <c r="AP70" s="10">
         <v>0</v>
       </c>
-      <c r="AQ70" s="11">
+      <c r="AQ70" s="20">
         <v>6</v>
       </c>
       <c r="AR70" s="12">
@@ -7221,13 +7211,13 @@
       <c r="D71" s="15">
         <v>0</v>
       </c>
-      <c r="E71" s="13">
+      <c r="E71" s="21">
         <v>8</v>
       </c>
       <c r="F71" s="14">
         <v>0</v>
       </c>
-      <c r="G71" s="15">
+      <c r="G71" s="25">
         <v>3</v>
       </c>
       <c r="H71" s="13">
@@ -7248,13 +7238,13 @@
       <c r="N71" s="15">
         <v>0</v>
       </c>
-      <c r="O71" s="13">
+      <c r="O71" s="21">
         <v>8</v>
       </c>
       <c r="P71" s="14">
         <v>0</v>
       </c>
-      <c r="Q71" s="15">
+      <c r="Q71" s="25">
         <v>3</v>
       </c>
       <c r="R71" s="13">
@@ -7275,13 +7265,13 @@
       <c r="X71" s="15">
         <v>0</v>
       </c>
-      <c r="Y71" s="13">
+      <c r="Y71" s="21">
         <v>8</v>
       </c>
       <c r="Z71" s="14">
         <v>0</v>
       </c>
-      <c r="AA71" s="15">
+      <c r="AA71" s="25">
         <v>3</v>
       </c>
       <c r="AB71" s="13">
@@ -7302,13 +7292,13 @@
       <c r="AO71" s="15">
         <v>0</v>
       </c>
-      <c r="AP71" s="13">
+      <c r="AP71" s="21">
         <v>8</v>
       </c>
       <c r="AQ71" s="14">
         <v>0</v>
       </c>
-      <c r="AR71" s="15">
+      <c r="AR71" s="25">
         <v>3</v>
       </c>
       <c r="AS71" s="13">
@@ -7334,7 +7324,7 @@
       <c r="E72" s="16">
         <v>0</v>
       </c>
-      <c r="F72" s="17">
+      <c r="F72" s="22">
         <v>2</v>
       </c>
       <c r="G72" s="18">
@@ -7361,7 +7351,7 @@
       <c r="O72" s="16">
         <v>0</v>
       </c>
-      <c r="P72" s="17">
+      <c r="P72" s="22">
         <v>2</v>
       </c>
       <c r="Q72" s="18">
@@ -7388,7 +7378,7 @@
       <c r="Y72" s="16">
         <v>0</v>
       </c>
-      <c r="Z72" s="17">
+      <c r="Z72" s="22">
         <v>2</v>
       </c>
       <c r="AA72" s="18">
@@ -7400,7 +7390,7 @@
       <c r="AC72" s="17">
         <v>0</v>
       </c>
-      <c r="AD72" s="41">
+      <c r="AD72" s="40">
         <v>6</v>
       </c>
       <c r="AM72" s="27">
@@ -7415,7 +7405,7 @@
       <c r="AP72" s="16">
         <v>0</v>
       </c>
-      <c r="AQ72" s="17">
+      <c r="AQ72" s="22">
         <v>2</v>
       </c>
       <c r="AR72" s="18">
@@ -7762,41 +7752,41 @@
       </c>
     </row>
     <row r="78" spans="2:47" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="37"/>
-      <c r="I78" s="37"/>
-      <c r="J78" s="37"/>
-      <c r="K78" s="37"/>
-      <c r="L78" s="37"/>
-      <c r="M78" s="37"/>
-      <c r="N78" s="37"/>
-      <c r="O78" s="37"/>
-      <c r="P78" s="37"/>
-      <c r="Q78" s="37"/>
-      <c r="R78" s="37"/>
-      <c r="S78" s="37"/>
-      <c r="T78" s="37"/>
-      <c r="U78" s="37"/>
-      <c r="V78" s="37"/>
-      <c r="W78" s="37"/>
-      <c r="X78" s="37"/>
-      <c r="Y78" s="37"/>
-      <c r="Z78" s="37"/>
-      <c r="AA78" s="37"/>
-      <c r="AB78" s="37"/>
-      <c r="AC78" s="37"/>
-      <c r="AD78" s="37"/>
-      <c r="AE78" s="37"/>
-      <c r="AF78" s="37"/>
-      <c r="AG78" s="37"/>
-      <c r="AH78" s="37"/>
-      <c r="AI78" s="37"/>
-      <c r="AJ78" s="37"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="36"/>
+      <c r="I78" s="36"/>
+      <c r="J78" s="36"/>
+      <c r="K78" s="36"/>
+      <c r="L78" s="36"/>
+      <c r="M78" s="36"/>
+      <c r="N78" s="36"/>
+      <c r="O78" s="36"/>
+      <c r="P78" s="36"/>
+      <c r="Q78" s="36"/>
+      <c r="R78" s="36"/>
+      <c r="S78" s="36"/>
+      <c r="T78" s="36"/>
+      <c r="U78" s="36"/>
+      <c r="V78" s="36"/>
+      <c r="W78" s="36"/>
+      <c r="X78" s="36"/>
+      <c r="Y78" s="36"/>
+      <c r="Z78" s="36"/>
+      <c r="AA78" s="36"/>
+      <c r="AB78" s="36"/>
+      <c r="AC78" s="36"/>
+      <c r="AD78" s="36"/>
+      <c r="AE78" s="36"/>
+      <c r="AF78" s="36"/>
+      <c r="AG78" s="36"/>
+      <c r="AH78" s="36"/>
+      <c r="AI78" s="36"/>
+      <c r="AJ78" s="36"/>
     </row>
     <row r="80" spans="2:47" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="81" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7919,7 +7909,7 @@
       <c r="N82" s="15">
         <v>0</v>
       </c>
-      <c r="O82" s="39">
+      <c r="O82" s="38">
         <v>1</v>
       </c>
       <c r="P82" s="24">
@@ -8061,7 +8051,7 @@
       <c r="E84" s="10">
         <v>0</v>
       </c>
-      <c r="F84" s="11">
+      <c r="F84" s="20">
         <v>6</v>
       </c>
       <c r="G84" s="12">
@@ -8088,7 +8078,7 @@
       <c r="O84" s="10">
         <v>0</v>
       </c>
-      <c r="P84" s="11">
+      <c r="P84" s="20">
         <v>6</v>
       </c>
       <c r="Q84" s="12">
@@ -8115,7 +8105,7 @@
       <c r="Y84" s="10">
         <v>0</v>
       </c>
-      <c r="Z84" s="11">
+      <c r="Z84" s="20">
         <v>6</v>
       </c>
       <c r="AA84" s="12">
@@ -8141,13 +8131,13 @@
       <c r="D85" s="15">
         <v>0</v>
       </c>
-      <c r="E85" s="13">
+      <c r="E85" s="21">
         <v>8</v>
       </c>
       <c r="F85" s="14">
         <v>0</v>
       </c>
-      <c r="G85" s="15">
+      <c r="G85" s="25">
         <v>3</v>
       </c>
       <c r="H85" s="13">
@@ -8168,13 +8158,13 @@
       <c r="N85" s="15">
         <v>0</v>
       </c>
-      <c r="O85" s="13">
+      <c r="O85" s="21">
         <v>8</v>
       </c>
       <c r="P85" s="14">
         <v>0</v>
       </c>
-      <c r="Q85" s="15">
+      <c r="Q85" s="25">
         <v>3</v>
       </c>
       <c r="R85" s="13">
@@ -8195,13 +8185,13 @@
       <c r="X85" s="15">
         <v>0</v>
       </c>
-      <c r="Y85" s="13">
+      <c r="Y85" s="21">
         <v>8</v>
       </c>
       <c r="Z85" s="14">
         <v>0</v>
       </c>
-      <c r="AA85" s="15">
+      <c r="AA85" s="25">
         <v>3</v>
       </c>
       <c r="AB85" s="13">
@@ -8227,7 +8217,7 @@
       <c r="E86" s="16">
         <v>0</v>
       </c>
-      <c r="F86" s="17">
+      <c r="F86" s="22">
         <v>2</v>
       </c>
       <c r="G86" s="18">
@@ -8254,7 +8244,7 @@
       <c r="O86" s="16">
         <v>0</v>
       </c>
-      <c r="P86" s="17">
+      <c r="P86" s="22">
         <v>2</v>
       </c>
       <c r="Q86" s="18">
@@ -8281,7 +8271,7 @@
       <c r="Y86" s="16">
         <v>0</v>
       </c>
-      <c r="Z86" s="17">
+      <c r="Z86" s="22">
         <v>2</v>
       </c>
       <c r="AA86" s="18">
@@ -8728,7 +8718,7 @@
       <c r="E94" s="10">
         <v>0</v>
       </c>
-      <c r="F94" s="11">
+      <c r="F94" s="20">
         <v>6</v>
       </c>
       <c r="G94" s="12">
@@ -8755,7 +8745,7 @@
       <c r="O94" s="10">
         <v>0</v>
       </c>
-      <c r="P94" s="11">
+      <c r="P94" s="20">
         <v>6</v>
       </c>
       <c r="Q94" s="12">
@@ -8781,13 +8771,13 @@
       <c r="D95" s="15">
         <v>0</v>
       </c>
-      <c r="E95" s="13">
+      <c r="E95" s="21">
         <v>8</v>
       </c>
       <c r="F95" s="14">
         <v>0</v>
       </c>
-      <c r="G95" s="15">
+      <c r="G95" s="25">
         <v>3</v>
       </c>
       <c r="H95" s="13">
@@ -8808,13 +8798,13 @@
       <c r="N95" s="15">
         <v>0</v>
       </c>
-      <c r="O95" s="13">
+      <c r="O95" s="21">
         <v>8</v>
       </c>
       <c r="P95" s="14">
         <v>0</v>
       </c>
-      <c r="Q95" s="15">
+      <c r="Q95" s="25">
         <v>3</v>
       </c>
       <c r="R95" s="13">
@@ -8840,7 +8830,7 @@
       <c r="E96" s="16">
         <v>0</v>
       </c>
-      <c r="F96" s="17">
+      <c r="F96" s="22">
         <v>2</v>
       </c>
       <c r="G96" s="18">
@@ -8867,7 +8857,7 @@
       <c r="O96" s="16">
         <v>0</v>
       </c>
-      <c r="P96" s="17">
+      <c r="P96" s="22">
         <v>2</v>
       </c>
       <c r="Q96" s="18">
@@ -9052,54 +9042,54 @@
       </c>
     </row>
     <row r="101" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="36"/>
-      <c r="C101" s="36"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="36"/>
-      <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
-      <c r="K101" s="36"/>
-      <c r="L101" s="36"/>
-      <c r="M101" s="36"/>
-      <c r="N101" s="36"/>
-      <c r="O101" s="36"/>
-      <c r="P101" s="36"/>
-      <c r="Q101" s="36"/>
-      <c r="R101" s="36"/>
-      <c r="S101" s="36"/>
-      <c r="T101" s="36"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="35"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="35"/>
+      <c r="F101" s="35"/>
+      <c r="G101" s="35"/>
+      <c r="H101" s="35"/>
+      <c r="I101" s="35"/>
+      <c r="J101" s="35"/>
+      <c r="K101" s="35"/>
+      <c r="L101" s="35"/>
+      <c r="M101" s="35"/>
+      <c r="N101" s="35"/>
+      <c r="O101" s="35"/>
+      <c r="P101" s="35"/>
+      <c r="Q101" s="35"/>
+      <c r="R101" s="35"/>
+      <c r="S101" s="35"/>
+      <c r="T101" s="35"/>
     </row>
     <row r="102" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="37"/>
-      <c r="C102" s="37"/>
-      <c r="D102" s="37"/>
-      <c r="E102" s="37"/>
-      <c r="F102" s="37"/>
-      <c r="G102" s="37"/>
-      <c r="H102" s="37"/>
-      <c r="I102" s="37"/>
-      <c r="J102" s="37"/>
-      <c r="K102" s="37"/>
-      <c r="L102" s="37"/>
-      <c r="M102" s="37"/>
-      <c r="N102" s="37"/>
-      <c r="O102" s="37"/>
-      <c r="P102" s="37"/>
-      <c r="Q102" s="37"/>
-      <c r="R102" s="37"/>
-      <c r="S102" s="37"/>
-      <c r="T102" s="37"/>
-      <c r="U102" s="37"/>
-      <c r="V102" s="37"/>
-      <c r="W102" s="37"/>
-      <c r="X102" s="37"/>
-      <c r="Y102" s="37"/>
-      <c r="Z102" s="37"/>
-      <c r="AA102" s="37"/>
-      <c r="AB102" s="37"/>
+      <c r="B102" s="36"/>
+      <c r="C102" s="36"/>
+      <c r="D102" s="36"/>
+      <c r="E102" s="36"/>
+      <c r="F102" s="36"/>
+      <c r="G102" s="36"/>
+      <c r="H102" s="36"/>
+      <c r="I102" s="36"/>
+      <c r="J102" s="36"/>
+      <c r="K102" s="36"/>
+      <c r="L102" s="36"/>
+      <c r="M102" s="36"/>
+      <c r="N102" s="36"/>
+      <c r="O102" s="36"/>
+      <c r="P102" s="36"/>
+      <c r="Q102" s="36"/>
+      <c r="R102" s="36"/>
+      <c r="S102" s="36"/>
+      <c r="T102" s="36"/>
+      <c r="U102" s="36"/>
+      <c r="V102" s="36"/>
+      <c r="W102" s="36"/>
+      <c r="X102" s="36"/>
+      <c r="Y102" s="36"/>
+      <c r="Z102" s="36"/>
+      <c r="AA102" s="36"/>
+      <c r="AB102" s="36"/>
     </row>
     <row r="104" spans="2:28" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="105" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9283,7 +9273,7 @@
       <c r="E108" s="10">
         <v>0</v>
       </c>
-      <c r="F108" s="11">
+      <c r="F108" s="20">
         <v>6</v>
       </c>
       <c r="G108" s="12">
@@ -9310,7 +9300,7 @@
       <c r="O108" s="10">
         <v>0</v>
       </c>
-      <c r="P108" s="11">
+      <c r="P108" s="20">
         <v>6</v>
       </c>
       <c r="Q108" s="12">
@@ -9336,13 +9326,13 @@
       <c r="D109" s="15">
         <v>0</v>
       </c>
-      <c r="E109" s="13">
+      <c r="E109" s="21">
         <v>8</v>
       </c>
       <c r="F109" s="14">
         <v>0</v>
       </c>
-      <c r="G109" s="15">
+      <c r="G109" s="25">
         <v>3</v>
       </c>
       <c r="H109" s="13">
@@ -9363,13 +9353,13 @@
       <c r="N109" s="15">
         <v>0</v>
       </c>
-      <c r="O109" s="13">
+      <c r="O109" s="21">
         <v>8</v>
       </c>
       <c r="P109" s="14">
         <v>0</v>
       </c>
-      <c r="Q109" s="15">
+      <c r="Q109" s="25">
         <v>3</v>
       </c>
       <c r="R109" s="13">
@@ -9395,7 +9385,7 @@
       <c r="E110" s="16">
         <v>0</v>
       </c>
-      <c r="F110" s="17">
+      <c r="F110" s="22">
         <v>2</v>
       </c>
       <c r="G110" s="18">
@@ -9422,7 +9412,7 @@
       <c r="O110" s="16">
         <v>0</v>
       </c>
-      <c r="P110" s="17">
+      <c r="P110" s="22">
         <v>2</v>
       </c>
       <c r="Q110" s="18">
@@ -9650,7 +9640,7 @@
       <c r="P116" s="20">
         <v>7</v>
       </c>
-      <c r="Q116" s="38">
+      <c r="Q116" s="37">
         <v>1</v>
       </c>
       <c r="R116" s="10">
@@ -9869,7 +9859,7 @@
       <c r="E119" s="10">
         <v>0</v>
       </c>
-      <c r="F119" s="11">
+      <c r="F119" s="20">
         <v>6</v>
       </c>
       <c r="G119" s="12">
@@ -9896,7 +9886,7 @@
       <c r="O119" s="10">
         <v>0</v>
       </c>
-      <c r="P119" s="11">
+      <c r="P119" s="20">
         <v>6</v>
       </c>
       <c r="Q119" s="12">
@@ -9923,7 +9913,7 @@
       <c r="Y119" s="10">
         <v>0</v>
       </c>
-      <c r="Z119" s="11">
+      <c r="Z119" s="20">
         <v>6</v>
       </c>
       <c r="AA119" s="12">
@@ -9949,13 +9939,13 @@
       <c r="D120" s="15">
         <v>0</v>
       </c>
-      <c r="E120" s="13">
+      <c r="E120" s="21">
         <v>8</v>
       </c>
       <c r="F120" s="14">
         <v>0</v>
       </c>
-      <c r="G120" s="15">
+      <c r="G120" s="25">
         <v>3</v>
       </c>
       <c r="H120" s="13">
@@ -9976,13 +9966,13 @@
       <c r="N120" s="15">
         <v>0</v>
       </c>
-      <c r="O120" s="13">
+      <c r="O120" s="21">
         <v>8</v>
       </c>
       <c r="P120" s="14">
         <v>0</v>
       </c>
-      <c r="Q120" s="15">
+      <c r="Q120" s="25">
         <v>3</v>
       </c>
       <c r="R120" s="13">
@@ -10003,13 +9993,13 @@
       <c r="X120" s="15">
         <v>0</v>
       </c>
-      <c r="Y120" s="13">
+      <c r="Y120" s="21">
         <v>8</v>
       </c>
       <c r="Z120" s="14">
         <v>0</v>
       </c>
-      <c r="AA120" s="15">
+      <c r="AA120" s="25">
         <v>3</v>
       </c>
       <c r="AB120" s="13">
@@ -10035,7 +10025,7 @@
       <c r="E121" s="16">
         <v>0</v>
       </c>
-      <c r="F121" s="17">
+      <c r="F121" s="22">
         <v>2</v>
       </c>
       <c r="G121" s="18">
@@ -10062,7 +10052,7 @@
       <c r="O121" s="16">
         <v>0</v>
       </c>
-      <c r="P121" s="17">
+      <c r="P121" s="22">
         <v>2</v>
       </c>
       <c r="Q121" s="18">
@@ -10089,7 +10079,7 @@
       <c r="Y121" s="16">
         <v>0</v>
       </c>
-      <c r="Z121" s="17">
+      <c r="Z121" s="22">
         <v>2</v>
       </c>
       <c r="AA121" s="18">

</xml_diff>

<commit_message>
first iteration of lpsolve text
</commit_message>
<xml_diff>
--- a/recursive_map.xlsx
+++ b/recursive_map.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Custom_Projects\optimering_grupp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC65322A-09F6-45ED-BC69-3BCDF2E20AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCA7364-B9CE-4CB3-BDC5-F431D43F2C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E2015ED8-7778-4B4B-B55F-488E888CCD57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{E2015ED8-7778-4B4B-B55F-488E888CCD57}"/>
   </bookViews>
   <sheets>
     <sheet name="9x9" sheetId="2" r:id="rId1"/>
     <sheet name="3x3" sheetId="1" r:id="rId2"/>
+    <sheet name="images" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,19 +36,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>…...</t>
   </si>
   <si>
     <t>…..</t>
   </si>
+  <si>
+    <t>Easy sudoku02</t>
+  </si>
+  <si>
+    <t>Expert sudoku04</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +107,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,7 +282,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,6 +411,84 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1048,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D49F0B6-0387-4E66-8DC6-56828B3094F0}">
   <dimension ref="B1:CL124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL29" sqref="AL29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10819,4 +10912,870 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08A4182-F5BD-435D-92D9-9B9122FEF4E9}">
+  <dimension ref="B2:T26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:U27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+    </row>
+    <row r="3" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="44"/>
+      <c r="C4" s="20">
+        <v>8</v>
+      </c>
+      <c r="D4" s="26">
+        <v>3</v>
+      </c>
+      <c r="E4" s="44"/>
+      <c r="F4" s="20">
+        <v>2</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1</v>
+      </c>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="26">
+        <v>7</v>
+      </c>
+      <c r="L4" s="29">
+        <v>4</v>
+      </c>
+      <c r="M4" s="20">
+        <v>8</v>
+      </c>
+      <c r="N4" s="26">
+        <v>3</v>
+      </c>
+      <c r="O4" s="29">
+        <v>9</v>
+      </c>
+      <c r="P4" s="20">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>1</v>
+      </c>
+      <c r="R4" s="29">
+        <v>6</v>
+      </c>
+      <c r="S4" s="33">
+        <v>5</v>
+      </c>
+      <c r="T4" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21">
+        <v>9</v>
+      </c>
+      <c r="C5" s="24">
+        <v>6</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="21">
+        <v>3</v>
+      </c>
+      <c r="F5" s="48"/>
+      <c r="G5" s="25">
+        <v>5</v>
+      </c>
+      <c r="H5" s="21">
+        <v>8</v>
+      </c>
+      <c r="I5" s="24">
+        <v>2</v>
+      </c>
+      <c r="J5" s="25">
+        <v>1</v>
+      </c>
+      <c r="L5" s="21">
+        <v>9</v>
+      </c>
+      <c r="M5" s="24">
+        <v>6</v>
+      </c>
+      <c r="N5" s="60">
+        <v>7</v>
+      </c>
+      <c r="O5" s="21">
+        <v>3</v>
+      </c>
+      <c r="P5" s="57">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="25">
+        <v>5</v>
+      </c>
+      <c r="R5" s="21">
+        <v>8</v>
+      </c>
+      <c r="S5" s="24">
+        <v>2</v>
+      </c>
+      <c r="T5" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="27">
+        <v>2</v>
+      </c>
+      <c r="C6" s="22">
+        <v>5</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="23">
+        <v>6</v>
+      </c>
+      <c r="H6" s="49"/>
+      <c r="I6" s="22">
+        <v>9</v>
+      </c>
+      <c r="J6" s="23">
+        <v>3</v>
+      </c>
+      <c r="L6" s="27">
+        <v>2</v>
+      </c>
+      <c r="M6" s="22">
+        <v>5</v>
+      </c>
+      <c r="N6" s="23">
+        <v>1</v>
+      </c>
+      <c r="O6" s="56">
+        <v>8</v>
+      </c>
+      <c r="P6" s="58">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="23">
+        <v>6</v>
+      </c>
+      <c r="R6" s="56">
+        <v>4</v>
+      </c>
+      <c r="S6" s="22">
+        <v>9</v>
+      </c>
+      <c r="T6" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44"/>
+      <c r="C7" s="20">
+        <v>4</v>
+      </c>
+      <c r="D7" s="26">
+        <v>8</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1</v>
+      </c>
+      <c r="F7" s="45"/>
+      <c r="G7" s="26">
+        <v>2</v>
+      </c>
+      <c r="H7" s="46"/>
+      <c r="I7" s="24">
+        <v>7</v>
+      </c>
+      <c r="J7" s="47"/>
+      <c r="L7" s="29">
+        <v>5</v>
+      </c>
+      <c r="M7" s="20">
+        <v>4</v>
+      </c>
+      <c r="N7" s="26">
+        <v>8</v>
+      </c>
+      <c r="O7" s="19">
+        <v>1</v>
+      </c>
+      <c r="P7" s="33">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>2</v>
+      </c>
+      <c r="R7" s="57">
+        <v>9</v>
+      </c>
+      <c r="S7" s="24">
+        <v>7</v>
+      </c>
+      <c r="T7" s="60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="51"/>
+      <c r="C8" s="24">
+        <v>2</v>
+      </c>
+      <c r="D8" s="25">
+        <v>9</v>
+      </c>
+      <c r="E8" s="51"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="25">
+        <v>4</v>
+      </c>
+      <c r="H8" s="52"/>
+      <c r="I8" s="24">
+        <v>3</v>
+      </c>
+      <c r="J8" s="47"/>
+      <c r="L8" s="55">
+        <v>7</v>
+      </c>
+      <c r="M8" s="24">
+        <v>2</v>
+      </c>
+      <c r="N8" s="25">
+        <v>9</v>
+      </c>
+      <c r="O8" s="55">
+        <v>5</v>
+      </c>
+      <c r="P8" s="57">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="25">
+        <v>4</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
+      <c r="S8" s="24">
+        <v>3</v>
+      </c>
+      <c r="T8" s="60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="49"/>
+      <c r="C9" s="22">
+        <v>3</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="27">
+        <v>7</v>
+      </c>
+      <c r="F9" s="50"/>
+      <c r="G9" s="23">
+        <v>8</v>
+      </c>
+      <c r="H9" s="48"/>
+      <c r="I9" s="24">
+        <v>4</v>
+      </c>
+      <c r="J9" s="47"/>
+      <c r="L9" s="56">
+        <v>1</v>
+      </c>
+      <c r="M9" s="22">
+        <v>3</v>
+      </c>
+      <c r="N9" s="59">
+        <v>6</v>
+      </c>
+      <c r="O9" s="27">
+        <v>7</v>
+      </c>
+      <c r="P9" s="58">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>8</v>
+      </c>
+      <c r="R9" s="57">
+        <v>2</v>
+      </c>
+      <c r="S9" s="24">
+        <v>4</v>
+      </c>
+      <c r="T9" s="60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="19">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20">
+        <v>7</v>
+      </c>
+      <c r="D10" s="54"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="24">
+        <v>9</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="20">
+        <v>1</v>
+      </c>
+      <c r="J10" s="26">
+        <v>4</v>
+      </c>
+      <c r="L10" s="19">
+        <v>3</v>
+      </c>
+      <c r="M10" s="20">
+        <v>7</v>
+      </c>
+      <c r="N10" s="28">
+        <v>2</v>
+      </c>
+      <c r="O10" s="57">
+        <v>6</v>
+      </c>
+      <c r="P10" s="57">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="24">
+        <v>9</v>
+      </c>
+      <c r="R10" s="29">
+        <v>5</v>
+      </c>
+      <c r="S10" s="20">
+        <v>1</v>
+      </c>
+      <c r="T10" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21">
+        <v>8</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="24">
+        <v>2</v>
+      </c>
+      <c r="F11" s="24">
+        <v>5</v>
+      </c>
+      <c r="G11" s="24">
+        <v>3</v>
+      </c>
+      <c r="H11" s="51"/>
+      <c r="I11" s="24">
+        <v>6</v>
+      </c>
+      <c r="J11" s="25">
+        <v>9</v>
+      </c>
+      <c r="L11" s="21">
+        <v>8</v>
+      </c>
+      <c r="M11" s="24">
+        <v>1</v>
+      </c>
+      <c r="N11" s="60">
+        <v>4</v>
+      </c>
+      <c r="O11" s="24">
+        <v>2</v>
+      </c>
+      <c r="P11" s="24">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>3</v>
+      </c>
+      <c r="R11" s="55">
+        <v>7</v>
+      </c>
+      <c r="S11" s="24">
+        <v>6</v>
+      </c>
+      <c r="T11" s="25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="27">
+        <v>6</v>
+      </c>
+      <c r="C12" s="22">
+        <v>9</v>
+      </c>
+      <c r="D12" s="53"/>
+      <c r="E12" s="22">
+        <v>4</v>
+      </c>
+      <c r="F12" s="50">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
+        <v>7</v>
+      </c>
+      <c r="H12" s="49"/>
+      <c r="I12" s="22">
+        <v>8</v>
+      </c>
+      <c r="J12" s="23">
+        <v>2</v>
+      </c>
+      <c r="L12" s="27">
+        <v>6</v>
+      </c>
+      <c r="M12" s="22">
+        <v>9</v>
+      </c>
+      <c r="N12" s="59">
+        <v>5</v>
+      </c>
+      <c r="O12" s="22">
+        <v>4</v>
+      </c>
+      <c r="P12" s="58">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="22">
+        <v>7</v>
+      </c>
+      <c r="R12" s="56">
+        <v>3</v>
+      </c>
+      <c r="S12" s="22">
+        <v>8</v>
+      </c>
+      <c r="T12" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+    </row>
+    <row r="17" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="44"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="26">
+        <v>1</v>
+      </c>
+      <c r="E18" s="44"/>
+      <c r="F18" s="20">
+        <v>8</v>
+      </c>
+      <c r="G18" s="63"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="63"/>
+      <c r="L18" s="29">
+        <v>5</v>
+      </c>
+      <c r="M18" s="33">
+        <v>2</v>
+      </c>
+      <c r="N18" s="26">
+        <v>1</v>
+      </c>
+      <c r="O18" s="29">
+        <v>3</v>
+      </c>
+      <c r="P18" s="20">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="28">
+        <v>9</v>
+      </c>
+      <c r="R18" s="29">
+        <v>7</v>
+      </c>
+      <c r="S18" s="33">
+        <v>4</v>
+      </c>
+      <c r="T18" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="64"/>
+      <c r="C19" s="24">
+        <v>3</v>
+      </c>
+      <c r="D19" s="47"/>
+      <c r="E19" s="21">
+        <v>7</v>
+      </c>
+      <c r="F19" s="48"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="65"/>
+      <c r="L19" s="55">
+        <v>4</v>
+      </c>
+      <c r="M19" s="24">
+        <v>3</v>
+      </c>
+      <c r="N19" s="60">
+        <v>8</v>
+      </c>
+      <c r="O19" s="21">
+        <v>7</v>
+      </c>
+      <c r="P19" s="57">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="60">
+        <v>5</v>
+      </c>
+      <c r="R19" s="55">
+        <v>9</v>
+      </c>
+      <c r="S19" s="57">
+        <v>1</v>
+      </c>
+      <c r="T19" s="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="66"/>
+      <c r="C20" s="22">
+        <v>9</v>
+      </c>
+      <c r="D20" s="68"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="27">
+        <v>8</v>
+      </c>
+      <c r="I20" s="67"/>
+      <c r="J20" s="23">
+        <v>5</v>
+      </c>
+      <c r="L20" s="56">
+        <v>6</v>
+      </c>
+      <c r="M20" s="22">
+        <v>9</v>
+      </c>
+      <c r="N20" s="59">
+        <v>7</v>
+      </c>
+      <c r="O20" s="56">
+        <v>2</v>
+      </c>
+      <c r="P20" s="58">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="59">
+        <v>4</v>
+      </c>
+      <c r="R20" s="27">
+        <v>8</v>
+      </c>
+      <c r="S20" s="58">
+        <v>3</v>
+      </c>
+      <c r="T20" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="44"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="26">
+        <v>1</v>
+      </c>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="25">
+        <v>4</v>
+      </c>
+      <c r="L21" s="29">
+        <v>3</v>
+      </c>
+      <c r="M21" s="33">
+        <v>6</v>
+      </c>
+      <c r="N21" s="28">
+        <v>5</v>
+      </c>
+      <c r="O21" s="29">
+        <v>8</v>
+      </c>
+      <c r="P21" s="33">
+        <v>9</v>
+      </c>
+      <c r="Q21" s="26">
+        <v>1</v>
+      </c>
+      <c r="R21" s="57">
+        <v>2</v>
+      </c>
+      <c r="S21" s="57">
+        <v>7</v>
+      </c>
+      <c r="T21" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="51"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="25">
+        <v>3</v>
+      </c>
+      <c r="H22" s="52"/>
+      <c r="I22" s="24">
+        <v>9</v>
+      </c>
+      <c r="J22" s="25">
+        <v>1</v>
+      </c>
+      <c r="L22" s="55">
+        <v>8</v>
+      </c>
+      <c r="M22" s="57">
+        <v>7</v>
+      </c>
+      <c r="N22" s="60">
+        <v>2</v>
+      </c>
+      <c r="O22" s="55">
+        <v>4</v>
+      </c>
+      <c r="P22" s="57">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="25">
+        <v>3</v>
+      </c>
+      <c r="R22" s="2">
+        <v>6</v>
+      </c>
+      <c r="S22" s="24">
+        <v>9</v>
+      </c>
+      <c r="T22" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="49"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="27">
+        <v>6</v>
+      </c>
+      <c r="F23" s="22">
+        <v>7</v>
+      </c>
+      <c r="G23" s="23">
+        <v>2</v>
+      </c>
+      <c r="H23" s="48"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="47"/>
+      <c r="L23" s="56">
+        <v>1</v>
+      </c>
+      <c r="M23" s="58">
+        <v>4</v>
+      </c>
+      <c r="N23" s="59">
+        <v>9</v>
+      </c>
+      <c r="O23" s="27">
+        <v>6</v>
+      </c>
+      <c r="P23" s="22">
+        <v>7</v>
+      </c>
+      <c r="Q23" s="23">
+        <v>2</v>
+      </c>
+      <c r="R23" s="57">
+        <v>3</v>
+      </c>
+      <c r="S23" s="57">
+        <v>5</v>
+      </c>
+      <c r="T23" s="60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="19">
+        <v>7</v>
+      </c>
+      <c r="C24" s="62"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="24">
+        <v>3</v>
+      </c>
+      <c r="G24" s="46"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="20">
+        <v>2</v>
+      </c>
+      <c r="J24" s="63"/>
+      <c r="L24" s="19">
+        <v>7</v>
+      </c>
+      <c r="M24" s="33">
+        <v>8</v>
+      </c>
+      <c r="N24" s="28">
+        <v>4</v>
+      </c>
+      <c r="O24" s="57">
+        <v>1</v>
+      </c>
+      <c r="P24" s="24">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="57">
+        <v>6</v>
+      </c>
+      <c r="R24" s="29">
+        <v>5</v>
+      </c>
+      <c r="S24" s="20">
+        <v>2</v>
+      </c>
+      <c r="T24" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="21">
+        <v>2</v>
+      </c>
+      <c r="C25" s="46"/>
+      <c r="D25" s="25">
+        <v>6</v>
+      </c>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="21">
+        <v>1</v>
+      </c>
+      <c r="I25" s="46"/>
+      <c r="J25" s="65"/>
+      <c r="L25" s="21">
+        <v>2</v>
+      </c>
+      <c r="M25" s="57">
+        <v>5</v>
+      </c>
+      <c r="N25" s="25">
+        <v>6</v>
+      </c>
+      <c r="O25" s="57">
+        <v>9</v>
+      </c>
+      <c r="P25" s="57">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="57">
+        <v>7</v>
+      </c>
+      <c r="R25" s="21">
+        <v>1</v>
+      </c>
+      <c r="S25" s="57">
+        <v>8</v>
+      </c>
+      <c r="T25" s="60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="66"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="22">
+        <v>6</v>
+      </c>
+      <c r="J26" s="68"/>
+      <c r="L26" s="56">
+        <v>9</v>
+      </c>
+      <c r="M26" s="58">
+        <v>1</v>
+      </c>
+      <c r="N26" s="59">
+        <v>3</v>
+      </c>
+      <c r="O26" s="58">
+        <v>5</v>
+      </c>
+      <c r="P26" s="58">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="58">
+        <v>8</v>
+      </c>
+      <c r="R26" s="56">
+        <v>4</v>
+      </c>
+      <c r="S26" s="22">
+        <v>6</v>
+      </c>
+      <c r="T26" s="59">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J16:L16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>